<commit_message>
Update my_data.xlsx && combined_script_2.py
</commit_message>
<xml_diff>
--- a/Scripts/my_data.xlsx
+++ b/Scripts/my_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>name</t>
   </si>
@@ -49,7 +49,7 @@
     <t>row top-cat-block figure-wrapper</t>
   </si>
   <si>
-    <t>articleBody</t>
+    <t>content count-br</t>
   </si>
   <si>
     <t>true</t>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>nEjlO</t>
+  </si>
+  <si>
+    <t>_s30J clearfix</t>
   </si>
   <si>
     <t>false</t>
@@ -135,7 +138,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +163,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;Droid Sans Mono&quot;"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -224,10 +233,10 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -616,30 +625,30 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
@@ -647,22 +656,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
@@ -670,66 +679,66 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G7" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>12</v>

</xml_diff>